<commit_message>
modified sample sheet to fix a typeo
still trying to find what is different about hpgl0775, I thought I found
it but apparently not... hmmm
</commit_message>
<xml_diff>
--- a/sample_sheets/all_samples.xlsx
+++ b/sample_sheets/all_samples.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="148">
   <si>
     <t xml:space="preserve">Sample ID</t>
   </si>
@@ -116,6 +116,9 @@
     <t xml:space="preserve">wt ade2-1 can1-100 his3-11 leu2-3, 112 trp1-1 ura3-1 cbf5::TRP1 + CBF5 on pRS313</t>
   </si>
   <si>
+    <t xml:space="preserve">preprocessing/E1/hpgl0564/outputs/bowtie2_scerevisiae/hpgl0564_forward-trimmed.count.xz</t>
+  </si>
+  <si>
     <t xml:space="preserve">preprocessing/E1/hpgl0564/hpgl0564_scerevisiae.count.xz</t>
   </si>
   <si>
@@ -128,6 +131,9 @@
     <t xml:space="preserve">B</t>
   </si>
   <si>
+    <t xml:space="preserve">preprocessing/E1/hpgl0565/outputs/bowtie2_scerevisiae/hpgl0565_forward-trimmed.count.xz</t>
+  </si>
+  <si>
     <t xml:space="preserve">preprocessing/E1/hpgl0565/hpgl0565_scerevisiae.count.xz</t>
   </si>
   <si>
@@ -140,6 +146,9 @@
     <t xml:space="preserve">E</t>
   </si>
   <si>
+    <t xml:space="preserve">preprocessing/E1/hpgl0566/outputs/bowtie2_scerevisiae/hpgl0566_forward-trimmed.count.xz</t>
+  </si>
+  <si>
     <t xml:space="preserve">preprocessing/E1/hpgl0566/hpgl0566_scerevisiae.count.xz</t>
   </si>
   <si>
@@ -152,6 +161,9 @@
     <t xml:space="preserve">F</t>
   </si>
   <si>
+    <t xml:space="preserve">preprocessing/E1/hpgl0567/outputs/bowtie2_scerevisiae/hpgl0567_forward-trimmed.count.xz </t>
+  </si>
+  <si>
     <t xml:space="preserve">preprocessing/E1/hpgl0567/hpgl0567_scerevisiae.count.xz</t>
   </si>
   <si>
@@ -173,6 +185,9 @@
     <t xml:space="preserve">d95a ade2-1 can1-100 his3-11 leu2-3, 112 trp1-1 ura3-1 cbf5::TRP1 + CBF5 D95A on pRS313</t>
   </si>
   <si>
+    <t xml:space="preserve">preprocessing/E1/hpgl0568/outputs/bowtie2_scerevisiae/hpgl0568_forward-trimmed.count.xz </t>
+  </si>
+  <si>
     <t xml:space="preserve">preprocessing/E1/hpgl0568/hpgl0568_scerevisiae.count.xz</t>
   </si>
   <si>
@@ -185,6 +200,9 @@
     <t xml:space="preserve">C</t>
   </si>
   <si>
+    <t xml:space="preserve">preprocessing/E1/hpgl0569/outputs/bowtie2_scerevisiae/hpgl0569_forward-trimmed.count.xz </t>
+  </si>
+  <si>
     <t xml:space="preserve">preprocessing/E1/hpgl0569/hpgl0569_scerevisiae.count.xz</t>
   </si>
   <si>
@@ -197,6 +215,9 @@
     <t xml:space="preserve">D</t>
   </si>
   <si>
+    <t xml:space="preserve">preprocessing/E1/hpgl0570/outputs/bowtie2_scerevisiae/hpgl0570_forward-trimmed.count.xz </t>
+  </si>
+  <si>
     <t xml:space="preserve">preprocessing/E1/hpgl0570/hpgl0570_scerevisiae.count.xz</t>
   </si>
   <si>
@@ -206,6 +227,9 @@
     <t xml:space="preserve">SAMN09384247</t>
   </si>
   <si>
+    <t xml:space="preserve">preprocessing/E1/hpgl0571/outputs/bowtie2_scerevisiae/hpgl0571_forward-trimmed.count.xz </t>
+  </si>
+  <si>
     <t xml:space="preserve">preprocessing/E1/hpgl0571/hpgl0571_scerevisiae.count.xz</t>
   </si>
   <si>
@@ -224,30 +248,24 @@
     <t xml:space="preserve">18h</t>
   </si>
   <si>
-    <t xml:space="preserve">preprocessing/v2/hpgl0774/outputs/bowtie2_scerevisiae/hpgl0774_forward-trimmed.count.xz</t>
+    <t xml:space="preserve">preprocessing/E2/hpgl0774/outputs/bowtie2_scerevisiae/hpgl0774_forward-trimmed.count.xz</t>
   </si>
   <si>
     <t xml:space="preserve">preprocessing/E2/hpgl0774/outputs/bowtie2_scerevisiae/introns.count.xz</t>
   </si>
   <si>
-    <t xml:space="preserve">preprocessing/E2/hpgl0774/outputs/bowtie2_scerevisiae/hpgl0774_forward-trimmed.count.xz</t>
-  </si>
-  <si>
     <t xml:space="preserve">hpgl0775</t>
   </si>
   <si>
     <t xml:space="preserve">SAMN09384249</t>
   </si>
   <si>
-    <t xml:space="preserve">preprocessing/v2/hpgl0775/outputs/bowtie2_scerevisiae/hpgl0775_forward-trimmed.count.xz</t>
+    <t xml:space="preserve">preprocessing/E2/hpgl0775/outputs/bowtie2_scerevisiae/hpgl0775_forward-trimmed.count.xz</t>
   </si>
   <si>
     <t xml:space="preserve">preprocessing/E2/hpgl0775/outputs/bowtie2_scerevisiae/introns.count.xz</t>
   </si>
   <si>
-    <t xml:space="preserve">preprocessing/E2/hpgl0775/outputs/bowtie2_scerevisiae/hpgl0775_forward-trimmed.count.xz</t>
-  </si>
-  <si>
     <t xml:space="preserve">hpgl0776</t>
   </si>
   <si>
@@ -263,15 +281,12 @@
     <t xml:space="preserve">wt ade2-1 can1-100 his3-11 leu2-3, 112 trp1-1 ura3-1 cbf5::TRP1 upf1::LEU2 + CBF5 on pRS313 (yJD1524 upf1Δ)</t>
   </si>
   <si>
-    <t xml:space="preserve">preprocessing/v2/hpgl0776/outputs/bowtie2_scerevisiae/hpgl0776_forward-trimmed.count.xz</t>
+    <t xml:space="preserve">preprocessing/E2/hpgl0776/outputs/bowtie2_scerevisiae/hpgl0776_forward-trimmed.count.xz</t>
   </si>
   <si>
     <t xml:space="preserve">preprocessing/E2/hpgl0776/outputs/bowtie2_scerevisiae/introns.count.xz</t>
   </si>
   <si>
-    <t xml:space="preserve">preprocessing/E2/hpgl0776/outputs/bowtie2_scerevisiae/hpgl0776_forward-trimmed.count.xz</t>
-  </si>
-  <si>
     <t xml:space="preserve">hpgl0777</t>
   </si>
   <si>
@@ -287,15 +302,12 @@
     <t xml:space="preserve">d95a ade2-1 can1-100 his3-11 leu2-3, 112 trp1-1 ura3-1 cbf5::TRP1 upf1::LEU2 + CBF5 D95A on pRS313 (yJD1525 upf1Δ)</t>
   </si>
   <si>
-    <t xml:space="preserve">preprocessing/v2/hpgl0777/outputs/bowtie2_scerevisiae/hpgl0777_forward-trimmed.count.xz</t>
+    <t xml:space="preserve">preprocessing/E2/hpgl0777/outputs/bowtie2_scerevisiae/hpgl0777_forward-trimmed.count.xz</t>
   </si>
   <si>
     <t xml:space="preserve">preprocessing/E2/hpgl0777/outputs/bowtie2_scerevisiae/introns.count.xz</t>
   </si>
   <si>
-    <t xml:space="preserve">preprocessing/E2/hpgl0777/outputs/bowtie2_scerevisiae/hpgl0777_forward-trimmed.count.xz</t>
-  </si>
-  <si>
     <t xml:space="preserve">hpgl0778</t>
   </si>
   <si>
@@ -305,28 +317,22 @@
     <t xml:space="preserve">g</t>
   </si>
   <si>
-    <t xml:space="preserve">preprocessing/v2/hpgl0778/outputs/bowtie2_scerevisiae/hpgl0778_forward-trimmed.count.xz</t>
+    <t xml:space="preserve">preprocessing/E2/hpgl0778/outputs/bowtie2_scerevisiae/hpgl0778_forward-trimmed.count.xz</t>
   </si>
   <si>
     <t xml:space="preserve">preprocessing/E2/hpgl0778/outputs/bowtie2_scerevisiae/introns.count.xz</t>
   </si>
   <si>
-    <t xml:space="preserve">preprocessing/E2/hpgl0778/outputs/bowtie2_scerevisiae/hpgl0778_forward-trimmed.count.xz</t>
-  </si>
-  <si>
     <t xml:space="preserve">hpgl0779</t>
   </si>
   <si>
     <t xml:space="preserve">SAMN09384253</t>
   </si>
   <si>
-    <t xml:space="preserve">preprocessing/v2/hpgl0779/outputs/bowtie2_scerevisiae/hpgl0779_forward-trimmed.count.xz</t>
+    <t xml:space="preserve">preprocessing/E2/hpgl0779/outputs/bowtie2_scerevisiae/hpgl0779_forward-trimmed.count.xz</t>
   </si>
   <si>
     <t xml:space="preserve">preprocessing/E2/hpgl0779/outputs/bowtie2_scerevisiae/introns.count.xz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">preprocessing/E2/hpgl0779/outputs/bowtie2_scerevisiae/hpgl0779_forward-trimmed.count.xz</t>
   </si>
   <si>
     <t xml:space="preserve">hpgl0780</t>
@@ -357,30 +363,24 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">preprocessing/v2/hpgl0780/outputs/bowtie2_scerevisiae/hpgl0780_forward-trimmed.count.xz</t>
+    <t xml:space="preserve">preprocessing/E2/hpgl0780/outputs/bowtie2_scerevisiae/hpgl0780_forward-trimmed.count.xz</t>
   </si>
   <si>
     <t xml:space="preserve">preprocessing/E2/hpgl0780/outputs/bowtie2_scerevisiae/introns.count.xz</t>
   </si>
   <si>
-    <t xml:space="preserve">preprocessing/E2/hpgl0780/outputs/bowtie2_scerevisiae/hpgl0780_forward-trimmed.count.xz</t>
-  </si>
-  <si>
     <t xml:space="preserve">hpgl0781</t>
   </si>
   <si>
     <t xml:space="preserve">SAMN09384255</t>
   </si>
   <si>
-    <t xml:space="preserve">preprocessing/v2/hpgl0781/outputs/bowtie2_scerevisiae/hpgl0781_forward-trimmed.count.xz</t>
+    <t xml:space="preserve">preprocessing/E2/hpgl0781/outputs/bowtie2_scerevisiae/hpgl0781_forward-trimmed.count.xz</t>
   </si>
   <si>
     <t xml:space="preserve">preprocessing/E2/hpgl0781/outputs/bowtie2_scerevisiae/introns.count.xz</t>
   </si>
   <si>
-    <t xml:space="preserve">preprocessing/E2/hpgl0781/outputs/bowtie2_scerevisiae/hpgl0781_forward-trimmed.count.xz</t>
-  </si>
-  <si>
     <t xml:space="preserve">hpgl0782</t>
   </si>
   <si>
@@ -393,15 +393,12 @@
     <t xml:space="preserve">h</t>
   </si>
   <si>
-    <t xml:space="preserve">preprocessing/v2/hpgl0782/outputs/bowtie2_scerevisiae/hpgl0782_forward-trimmed.count.xz</t>
+    <t xml:space="preserve">preprocessing/E2/hpgl0782/outputs/bowtie2_scerevisiae/hpgl0782_forward-trimmed.count.xz</t>
   </si>
   <si>
     <t xml:space="preserve">preprocessing/E2/hpgl0782/outputs/bowtie2_scerevisiae/introns.count.xz</t>
   </si>
   <si>
-    <t xml:space="preserve">preprocessing/E2/hpgl0782/outputs/bowtie2_scerevisiae/hpgl0782_forward-trimmed.count.xz</t>
-  </si>
-  <si>
     <t xml:space="preserve">hpgl0783</t>
   </si>
   <si>
@@ -411,45 +408,36 @@
     <t xml:space="preserve">42h</t>
   </si>
   <si>
-    <t xml:space="preserve">preprocessing/v2/hpgl0783/outputs/bowtie2_scerevisiae/hpgl0783_forward-trimmed.count.xz</t>
+    <t xml:space="preserve">preprocessing/E2/hpgl0783/outputs/bowtie2_scerevisiae/hpgl0783_forward-trimmed.count.xz</t>
   </si>
   <si>
     <t xml:space="preserve">preprocessing/E2/hpgl0783/outputs/bowtie2_scerevisiae/introns.count.xz</t>
   </si>
   <si>
-    <t xml:space="preserve">preprocessing/E2/hpgl0783/outputs/bowtie2_scerevisiae/hpgl0783_forward-trimmed.count.xz</t>
-  </si>
-  <si>
     <t xml:space="preserve">hpgl0784</t>
   </si>
   <si>
     <t xml:space="preserve">SAMN09384258</t>
   </si>
   <si>
-    <t xml:space="preserve">preprocessing/v2/hpgl0784/outputs/bowtie2_scerevisiae/hpgl0784_forward-trimmed.count.xz</t>
+    <t xml:space="preserve">preprocessing/E2/hpgl0784/outputs/bowtie2_scerevisiae/hpgl0784_forward-trimmed.count.xz</t>
   </si>
   <si>
     <t xml:space="preserve">preprocessing/E2/hpgl0784/outputs/bowtie2_scerevisiae/introns.count.xz</t>
   </si>
   <si>
-    <t xml:space="preserve">preprocessing/E2/hpgl0784/outputs/bowtie2_scerevisiae/hpgl0784_forward-trimmed.count.xz</t>
-  </si>
-  <si>
     <t xml:space="preserve">hpgl0785</t>
   </si>
   <si>
     <t xml:space="preserve">SAMN09384259</t>
   </si>
   <si>
-    <t xml:space="preserve">preprocessing/v2/hpgl0785/outputs/bowtie2_scerevisiae/hpgl0785_forward-trimmed.count.xz</t>
+    <t xml:space="preserve">preprocessing/E2/hpgl0785/outputs/bowtie2_scerevisiae/hpgl0785_forward-trimmed.count.xz</t>
   </si>
   <si>
     <t xml:space="preserve">preprocessing/E2/hpgl0785/outputs/bowtie2_scerevisiae/introns.count.xz</t>
   </si>
   <si>
-    <t xml:space="preserve">preprocessing/E2/hpgl0785/outputs/bowtie2_scerevisiae/hpgl0785_forward-trimmed.count.xz</t>
-  </si>
-  <si>
     <t xml:space="preserve">hpgl0786</t>
   </si>
   <si>
@@ -459,58 +447,46 @@
     <t xml:space="preserve">I</t>
   </si>
   <si>
-    <t xml:space="preserve">preprocessing/v2/hpgl0786/outputs/bowtie2_scerevisiae/hpgl0786_forward-trimmed.count.xz</t>
+    <t xml:space="preserve">preprocessing/E2/hpgl0786/outputs/bowtie2_scerevisiae/hpgl0786_forward-trimmed.count.xz</t>
   </si>
   <si>
     <t xml:space="preserve">preprocessing/E2/hpgl0786/outputs/bowtie2_scerevisiae/introns.count.xz</t>
   </si>
   <si>
-    <t xml:space="preserve">preprocessing/E2/hpgl0786/outputs/bowtie2_scerevisiae/hpgl0786_forward-trimmed.count.xz</t>
-  </si>
-  <si>
     <t xml:space="preserve">hpgl0787</t>
   </si>
   <si>
     <t xml:space="preserve">SAMN09384261</t>
   </si>
   <si>
-    <t xml:space="preserve">preprocessing/v2/hpgl0787/outputs/bowtie2_scerevisiae/hpgl0787_forward-trimmed.count.xz</t>
+    <t xml:space="preserve">preprocessing/E2/hpgl0787/outputs/bowtie2_scerevisiae/hpgl0787_forward-trimmed.count.xz</t>
   </si>
   <si>
     <t xml:space="preserve">preprocessing/E2/hpgl0787/outputs/bowtie2_scerevisiae/introns.count.xz</t>
   </si>
   <si>
-    <t xml:space="preserve">preprocessing/E2/hpgl0787/outputs/bowtie2_scerevisiae/hpgl0787_forward-trimmed.count.xz</t>
-  </si>
-  <si>
     <t xml:space="preserve">hpgl0788</t>
   </si>
   <si>
     <t xml:space="preserve">SAMN09384262</t>
   </si>
   <si>
-    <t xml:space="preserve">preprocessing/v2/hpgl0788/outputs/bowtie2_scerevisiae/hpgl0788_forward-trimmed.count.xz</t>
+    <t xml:space="preserve">preprocessing/E2/hpgl0788/outputs/bowtie2_scerevisiae/hpgl0788_forward-trimmed.count.xz</t>
   </si>
   <si>
     <t xml:space="preserve">preprocessing/E2/hpgl0788/outputs/bowtie2_scerevisiae/introns.count.xz</t>
   </si>
   <si>
-    <t xml:space="preserve">preprocessing/E2/hpgl0788/outputs/bowtie2_scerevisiae/hpgl0788_forward-trimmed.count.xz</t>
-  </si>
-  <si>
     <t xml:space="preserve">hpgl0789</t>
   </si>
   <si>
     <t xml:space="preserve">SAMN09384263</t>
   </si>
   <si>
-    <t xml:space="preserve">preprocessing/v2/hpgl0789/outputs/bowtie2_scerevisiae/hpgl0789_forward-trimmed.count.xz</t>
+    <t xml:space="preserve">preprocessing/E2/hpgl0789/outputs/bowtie2_scerevisiae/hpgl0789_forward-trimmed.count.xz</t>
   </si>
   <si>
     <t xml:space="preserve">preprocessing/E2/hpgl0789/outputs/bowtie2_scerevisiae/introns.count.xz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">preprocessing/E2/hpgl0789/outputs/bowtie2_scerevisiae/hpgl0789_forward-trimmed.count.xz</t>
   </si>
 </sst>
 </file>
@@ -635,8 +611,8 @@
   </sheetPr>
   <dimension ref="A1:R28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="246" zoomScaleNormal="246" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="246" zoomScaleNormal="246" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P12" activeCellId="0" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -784,16 +760,19 @@
       <c r="O5" s="2" t="n">
         <v>6640227</v>
       </c>
+      <c r="P5" s="1" t="s">
+        <v>30</v>
+      </c>
       <c r="R5" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>23</v>
@@ -805,7 +784,7 @@
         <v>25</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>27</v>
@@ -834,16 +813,19 @@
       <c r="O6" s="2" t="n">
         <v>4328605</v>
       </c>
+      <c r="P6" s="1" t="s">
+        <v>35</v>
+      </c>
       <c r="R6" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>23</v>
@@ -855,7 +837,7 @@
         <v>25</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>27</v>
@@ -884,16 +866,19 @@
       <c r="O7" s="2" t="n">
         <v>1764802</v>
       </c>
+      <c r="P7" s="1" t="s">
+        <v>40</v>
+      </c>
       <c r="R7" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>23</v>
@@ -905,7 +890,7 @@
         <v>25</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>27</v>
@@ -934,31 +919,34 @@
       <c r="O8" s="2" t="n">
         <v>5830493</v>
       </c>
+      <c r="P8" s="1" t="s">
+        <v>45</v>
+      </c>
       <c r="R8" s="1" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>27</v>
@@ -967,7 +955,7 @@
         <v>28</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="K9" s="3" t="n">
         <v>440.7</v>
@@ -984,31 +972,34 @@
       <c r="O9" s="2" t="n">
         <v>5358578</v>
       </c>
+      <c r="P9" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="R9" s="1" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>27</v>
@@ -1017,7 +1008,7 @@
         <v>28</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="K10" s="3" t="n">
         <v>423.5</v>
@@ -1034,31 +1025,34 @@
       <c r="O10" s="2" t="n">
         <v>2477941</v>
       </c>
+      <c r="P10" s="1" t="s">
+        <v>58</v>
+      </c>
       <c r="R10" s="1" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>27</v>
@@ -1067,7 +1061,7 @@
         <v>28</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="K11" s="3" t="n">
         <v>580.6</v>
@@ -1084,31 +1078,34 @@
       <c r="O11" s="2" t="n">
         <v>7038596</v>
       </c>
+      <c r="P11" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="R11" s="1" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>25</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>27</v>
@@ -1117,7 +1114,7 @@
         <v>28</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="K12" s="3" t="n">
         <v>433.8</v>
@@ -1134,16 +1131,19 @@
       <c r="O12" s="2" t="n">
         <v>2404857</v>
       </c>
+      <c r="P12" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="R12" s="1" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>23</v>
@@ -1152,10 +1152,10 @@
         <v>24</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>27</v>
@@ -1164,7 +1164,7 @@
         <v>27</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="J13" s="3" t="s">
         <v>29</v>
@@ -1182,45 +1182,45 @@
         <v>4097983</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>70</v>
+        <v>77</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="K14" s="3"/>
       <c r="L14" s="2" t="n">
@@ -1236,45 +1236,45 @@
         <v>6211230</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>27</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="K15" s="3"/>
       <c r="L15" s="2" t="n">
@@ -1290,45 +1290,45 @@
         <v>5030522</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="K16" s="3"/>
       <c r="L16" s="2" t="n">
@@ -1344,21 +1344,21 @@
         <v>6432988</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>23</v>
@@ -1367,10 +1367,10 @@
         <v>24</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>27</v>
@@ -1379,7 +1379,7 @@
         <v>27</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="J17" s="3" t="s">
         <v>29</v>
@@ -1397,45 +1397,45 @@
         <v>5310337</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="G18" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="K18" s="3"/>
       <c r="L18" s="2" t="n">
@@ -1451,45 +1451,45 @@
         <v>6202761</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>27</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="K19" s="3"/>
       <c r="L19" s="2" t="n">
@@ -1505,10 +1505,10 @@
         <v>4963385</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="R19" s="1" t="s">
         <v>106</v>
@@ -1516,34 +1516,34 @@
     </row>
     <row r="20" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="K20" s="3"/>
       <c r="L20" s="2" t="n">
@@ -1559,13 +1559,13 @@
         <v>5494737</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="Q20" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="R20" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="R20" s="1" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1594,7 +1594,7 @@
         <v>27</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="J21" s="3" t="s">
         <v>29</v>
@@ -1618,21 +1618,21 @@
         <v>117</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="B22" s="2" t="s">
-        <v>120</v>
-      </c>
       <c r="C22" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>114</v>
@@ -1641,16 +1641,16 @@
         <v>115</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="K22" s="3"/>
       <c r="L22" s="2" t="n">
@@ -1666,27 +1666,27 @@
         <v>7862561</v>
       </c>
       <c r="P22" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q22" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="Q22" s="1" t="s">
-        <v>123</v>
-      </c>
       <c r="R22" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>114</v>
@@ -1698,13 +1698,13 @@
         <v>27</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="J23" s="3" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="K23" s="3"/>
       <c r="L23" s="2" t="n">
@@ -1720,27 +1720,27 @@
         <v>6608579</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>114</v>
@@ -1749,16 +1749,16 @@
         <v>115</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J24" s="3" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="K24" s="3"/>
       <c r="L24" s="2" t="n">
@@ -1774,21 +1774,21 @@
         <v>8434812</v>
       </c>
       <c r="P24" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>23</v>
@@ -1800,7 +1800,7 @@
         <v>114</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>27</v>
@@ -1809,7 +1809,7 @@
         <v>27</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="J25" s="3" t="s">
         <v>29</v>
@@ -1827,45 +1827,45 @@
         <v>8442154</v>
       </c>
       <c r="P25" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="R25" s="1" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>114</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>27</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="K26" s="3"/>
       <c r="L26" s="2" t="n">
@@ -1881,45 +1881,45 @@
         <v>8423156</v>
       </c>
       <c r="P26" s="1" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="R26" s="1" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>114</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>27</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="J27" s="3" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="K27" s="3"/>
       <c r="L27" s="2" t="n">
@@ -1935,45 +1935,45 @@
         <v>8121054</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="R27" s="1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>114</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="K28" s="3"/>
       <c r="L28" s="2" t="n">
@@ -1989,13 +1989,13 @@
         <v>8486160</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="Q28" s="1" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="R28" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>